<commit_message>
More formulas on xlsx
</commit_message>
<xml_diff>
--- a/BMW Deal Finder.xlsx
+++ b/BMW Deal Finder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r0ot\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r0ot\git\bmwcrawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C39A6BE-2595-4B32-BFB6-C2AB983B16EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A9745D-D0A6-4509-8FDB-C31C21A4AB6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="6525" windowWidth="15870" windowHeight="17205" activeTab="1" xr2:uid="{50926F15-AF04-4611-A895-7A28EE78B717}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{50926F15-AF04-4611-A895-7A28EE78B717}"/>
   </bookViews>
   <sheets>
     <sheet name="RAWData" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="342">
   <si>
     <t>name</t>
   </si>
@@ -948,22 +948,7 @@
     <t>discountsales2077</t>
   </si>
   <si>
-    <t xml:space="preserve">
-2019
-330i xdrive</t>
-  </si>
-  <si>
-    <t>2020
-330i xdrive</t>
-  </si>
-  <si>
     <t>48,xxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020
-330i xdrive
-MSPORT
-</t>
   </si>
   <si>
     <t>54,xxx</t>
@@ -1106,10 +1091,6 @@
 Non M</t>
   </si>
   <si>
-    <t>530xi
-M Sport! Loaner</t>
-  </si>
-  <si>
     <t>330 xi Loaner</t>
   </si>
   <si>
@@ -1119,6 +1100,15 @@
     <t xml:space="preserve">X5 50i
 NEW
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">330i xdrive
+MSPORT
+</t>
+  </si>
+  <si>
+    <t>530xi 
+M Sport! Loaner</t>
   </si>
 </sst>
 </file>
@@ -1824,6 +1814,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2918,8 +2976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A842C1C-1518-4788-B002-5894EB90CE54}">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,7 +3025,7 @@
         <v>233</v>
       </c>
       <c r="F2" t="str">
-        <f>LEFT(A2,FIND(" ",A2)-1)</f>
+        <f t="shared" ref="F2:F46" si="0">IFERROR(LEFT(A2,FIND(" ",A2)-1),IFERROR(LEFT(A2,FIND(CHAR(10),A2)-1),A2))</f>
         <v>230i</v>
       </c>
       <c r="G2" t="str">
@@ -2992,7 +3050,7 @@
         <v>233</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="0">LEFT(A3,FIND(" ",A3)-1)</f>
+        <f t="shared" si="0"/>
         <v>230i</v>
       </c>
       <c r="G3" t="str">
@@ -3241,13 +3299,13 @@
       <c r="E13" t="s">
         <v>233</v>
       </c>
-      <c r="F13" t="e">
+      <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G13" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>M4</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>M4</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="81" thickBot="1" x14ac:dyDescent="0.4">
@@ -3391,13 +3449,13 @@
       <c r="E19" t="s">
         <v>233</v>
       </c>
-      <c r="F19" t="e">
+      <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>M5</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>M5</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -3968,13 +4026,13 @@
       <c r="E42" t="s">
         <v>233</v>
       </c>
-      <c r="F42" t="e">
+      <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G42" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>X3M</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>X3M</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4093,13 +4151,13 @@
       <c r="E47" t="s">
         <v>233</v>
       </c>
-      <c r="F47" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G47" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F47" t="str">
+        <f>IFERROR(LEFT(A47,FIND(" ",A47)-1),IFERROR(LEFT(A47,FIND(CHAR(10),A47)-1),A47))</f>
+        <v>X4M</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>X4M</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4119,7 +4177,7 @@
         <v>233</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F48:F81" si="2">IFERROR(LEFT(A48,FIND(" ",A48)-1),IFERROR(LEFT(A48,FIND(CHAR(10),A48)-1),A48))</f>
         <v>X4M</v>
       </c>
       <c r="G48" t="str">
@@ -4144,7 +4202,7 @@
         <v>233</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 X5</v>
       </c>
@@ -4171,7 +4229,7 @@
         <v>233</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 X5</v>
       </c>
@@ -4198,7 +4256,7 @@
         <v>233</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>X5</v>
       </c>
       <c r="G51" t="str">
@@ -4223,7 +4281,7 @@
         <v>233</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>X5</v>
       </c>
       <c r="G52" t="str">
@@ -4248,7 +4306,7 @@
         <v>233</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>X5</v>
       </c>
       <c r="G53" t="str">
@@ -4273,7 +4331,7 @@
         <v>233</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 X5M</v>
       </c>
@@ -4300,7 +4358,7 @@
         <v>233</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>x6</v>
       </c>
       <c r="G55" t="str">
@@ -4325,7 +4383,7 @@
         <v>233</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>x6</v>
       </c>
       <c r="G56" t="str">
@@ -4350,7 +4408,7 @@
         <v>233</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>X6M</v>
       </c>
       <c r="G57" t="str">
@@ -4375,7 +4433,7 @@
         <v>233</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>X7</v>
       </c>
       <c r="G58" t="str">
@@ -4400,7 +4458,7 @@
         <v>233</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 X7</v>
       </c>
@@ -4412,7 +4470,7 @@
     </row>
     <row r="60" spans="1:7" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="86" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B60" s="81">
         <v>41350</v>
@@ -4421,13 +4479,13 @@
         <v>0.13</v>
       </c>
       <c r="D60" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E60" t="s">
         <v>233</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>228xi</v>
       </c>
       <c r="G60" t="str">
@@ -4437,7 +4495,7 @@
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="87" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B61" s="83">
         <v>45200</v>
@@ -4446,23 +4504,23 @@
         <v>0.13</v>
       </c>
       <c r="D61" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E61" t="s">
         <v>233</v>
       </c>
-      <c r="F61" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G61" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F61" t="str">
+        <f t="shared" si="2"/>
+        <v>330xi</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="1"/>
+        <v>330</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="87" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B62" s="83">
         <v>58900</v>
@@ -4471,23 +4529,23 @@
         <v>0.13</v>
       </c>
       <c r="D62" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E62" t="s">
         <v>233</v>
       </c>
-      <c r="F62" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G62" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F62" t="str">
+        <f t="shared" si="2"/>
+        <v>530xi</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="1"/>
+        <v>530</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="86" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B63" s="81">
         <v>66550</v>
@@ -4496,23 +4554,23 @@
         <v>0.13</v>
       </c>
       <c r="D63" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E63" t="s">
         <v>233</v>
       </c>
-      <c r="F63" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G63" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F63" t="str">
+        <f t="shared" si="2"/>
+        <v>540xi</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="1"/>
+        <v>540</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="87" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B64" s="83">
         <v>79200</v>
@@ -4521,23 +4579,23 @@
         <v>0.123</v>
       </c>
       <c r="D64" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E64" t="s">
         <v>233</v>
       </c>
-      <c r="F64" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G64" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F64" t="str">
+        <f t="shared" si="2"/>
+        <v>M550xi</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="1"/>
+        <v>M550</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="86" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B65" s="81">
         <v>98300</v>
@@ -4546,23 +4604,23 @@
         <v>0.21</v>
       </c>
       <c r="D65" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E65" t="s">
         <v>233</v>
       </c>
-      <c r="F65" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G65" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F65" t="str">
+        <f t="shared" si="2"/>
+        <v>740xi</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="1"/>
+        <v>740</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="86" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B66" s="81">
         <v>93800</v>
@@ -4571,13 +4629,13 @@
         <v>0.15</v>
       </c>
       <c r="D66" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E66" t="s">
         <v>233</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>840xi</v>
       </c>
       <c r="G66" t="str">
@@ -4587,7 +4645,7 @@
     </row>
     <row r="67" spans="1:7" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="87" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B67" s="83">
         <v>150200</v>
@@ -4596,13 +4654,13 @@
         <v>0.2</v>
       </c>
       <c r="D67" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E67" t="s">
         <v>233</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F81" si="2">LEFT(A67,FIND(" ",A67)-1)</f>
+        <f t="shared" si="2"/>
         <v>M8</v>
       </c>
       <c r="G67" t="str">
@@ -4612,7 +4670,7 @@
     </row>
     <row r="68" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="86" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B68" s="81">
         <v>135900</v>
@@ -4621,7 +4679,7 @@
         <v>0.2</v>
       </c>
       <c r="D68" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E68" t="s">
         <v>233</v>
@@ -4637,7 +4695,7 @@
     </row>
     <row r="69" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="87" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B69" s="83">
         <v>54840</v>
@@ -4646,7 +4704,7 @@
         <v>0.13</v>
       </c>
       <c r="D69" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E69" t="s">
         <v>233</v>
@@ -4662,7 +4720,7 @@
     </row>
     <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="86" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B70" s="81">
         <v>83600</v>
@@ -4671,7 +4729,7 @@
         <v>0.125</v>
       </c>
       <c r="D70" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E70" t="s">
         <v>233</v>
@@ -4687,7 +4745,7 @@
     </row>
     <row r="71" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="86" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B71" s="81">
         <v>42900</v>
@@ -4696,7 +4754,7 @@
         <v>0.13</v>
       </c>
       <c r="D71" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E71" t="s">
         <v>233</v>
@@ -4712,7 +4770,7 @@
     </row>
     <row r="72" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="87" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B72" s="83">
         <v>46500</v>
@@ -4721,7 +4779,7 @@
         <v>0.13</v>
       </c>
       <c r="D72" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E72" t="s">
         <v>233</v>
@@ -4737,7 +4795,7 @@
     </row>
     <row r="73" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="86" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B73" s="81">
         <v>49500</v>
@@ -4746,7 +4804,7 @@
         <v>0.13</v>
       </c>
       <c r="D73" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E73" t="s">
         <v>233</v>
@@ -4771,18 +4829,18 @@
         <v>0.13</v>
       </c>
       <c r="D74" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E74" t="s">
         <v>233</v>
       </c>
-      <c r="F74" t="e">
+      <c r="F74" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G74" t="e">
+        <v>X3M</v>
+      </c>
+      <c r="G74" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>X3M</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -4796,7 +4854,7 @@
         <v>0.13</v>
       </c>
       <c r="D75" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E75" t="s">
         <v>233</v>
@@ -4821,23 +4879,23 @@
         <v>0.13</v>
       </c>
       <c r="D76" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E76" t="s">
         <v>233</v>
       </c>
-      <c r="F76" t="e">
+      <c r="F76" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G76" t="e">
+        <v>X4M</v>
+      </c>
+      <c r="G76" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>X4M</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="86" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B77" s="81">
         <v>62800</v>
@@ -4846,7 +4904,7 @@
         <v>0.13</v>
       </c>
       <c r="D77" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E77" t="s">
         <v>233</v>
@@ -4862,7 +4920,7 @@
     </row>
     <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="88" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B78" s="83">
         <v>94950</v>
@@ -4871,7 +4929,7 @@
         <v>0.125</v>
       </c>
       <c r="D78" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E78" t="s">
         <v>233</v>
@@ -4887,7 +4945,7 @@
     </row>
     <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="86" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B79" s="81">
         <v>123800</v>
@@ -4896,18 +4954,18 @@
         <v>0.06</v>
       </c>
       <c r="D79" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E79" t="s">
         <v>233</v>
       </c>
-      <c r="F79" t="e">
+      <c r="F79" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G79" t="e">
+        <v>X5M</v>
+      </c>
+      <c r="G79" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>X5M</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -4921,7 +4979,7 @@
         <v>0.13</v>
       </c>
       <c r="D80" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E80" t="s">
         <v>233</v>
@@ -4937,7 +4995,7 @@
     </row>
     <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="88" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B81" s="85">
         <v>101800</v>
@@ -4946,7 +5004,7 @@
         <v>0.125</v>
       </c>
       <c r="D81" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E81" t="s">
         <v>233</v>
@@ -4968,10 +5026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B7D44D-5CD3-45AB-906D-D9EB70CFB29F}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4979,7 +5037,7 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>227</v>
       </c>
@@ -4995,10 +5053,16 @@
       <c r="E1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="65.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="48" t="s">
-        <v>291</v>
+        <v>133</v>
       </c>
       <c r="B2" s="49" t="s">
         <v>189</v>
@@ -5012,13 +5076,21 @@
       <c r="E2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F2" t="str">
+        <f t="shared" ref="F2" si="0">IFERROR(LEFT(A2,FIND(" ",A2)-1),IFERROR(LEFT(A2,FIND(CHAR(10),A2)-1),A2))</f>
+        <v>330i</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(RIGHT(F2,1)="i",IF(RIGHT(F2,2)="xi",LEFT(F2,LEN(F2)-2),LEFT(F2,LEN(F2)-1)),F2)</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="51" t="s">
-        <v>292</v>
+        <v>133</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C3" s="9">
         <v>0.18</v>
@@ -5029,13 +5101,21 @@
       <c r="E3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="112.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F41" si="1">IFERROR(LEFT(A3,FIND(" ",A3)-1),IFERROR(LEFT(A3,FIND(CHAR(10),A3)-1),A3))</f>
+        <v>330i</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G41" si="2">IF(RIGHT(F3,1)="i",IF(RIGHT(F3,2)="xi",LEFT(F3,LEN(F3)-2),LEFT(F3,LEN(F3)-1)),F3)</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="96.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="53" t="s">
-        <v>294</v>
+        <v>340</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C4" s="55">
         <v>0.16400000000000001</v>
@@ -5046,13 +5126,21 @@
       <c r="E4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>330i</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="81" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="56" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C5" s="58">
         <v>0.17</v>
@@ -5063,13 +5151,21 @@
       <c r="E5" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>430i</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C6" s="60">
         <v>0.16</v>
@@ -5080,10 +5176,20 @@
       <c r="E6" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>2020
+530i</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>2020
+530</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="61" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B7" s="62" t="s">
         <v>189</v>
@@ -5097,13 +5203,21 @@
       <c r="E7" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>X2</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>X2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="61" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C8" s="9">
         <v>0.17</v>
@@ -5114,13 +5228,21 @@
       <c r="E8" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>X2</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>X2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="63" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C9" s="65">
         <v>0.17</v>
@@ -5131,10 +5253,20 @@
       <c r="E9" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>2020
+x3</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>2020
+x3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="63" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B10" s="64" t="s">
         <v>140</v>
@@ -5148,10 +5280,20 @@
       <c r="E10" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>2020
+x3</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>2020
+x3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="66" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B11" s="64" t="s">
         <v>136</v>
@@ -5165,13 +5307,23 @@
       <c r="E11" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>2020
+x3</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>2020
+x3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="53" t="s">
         <v>224</v>
       </c>
       <c r="B12" s="67" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C12" s="68">
         <v>0.17</v>
@@ -5182,8 +5334,16 @@
       <c r="E12" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>X7</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>X7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="69" t="s">
         <v>224</v>
       </c>
@@ -5199,42 +5359,66 @@
       <c r="E13" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>X7</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>X7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="72" t="s">
         <v>133</v>
       </c>
       <c r="B14" s="73" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C14" s="74">
         <v>0.19</v>
       </c>
       <c r="D14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E14" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>330i</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="75" t="s">
         <v>133</v>
       </c>
       <c r="B15" s="76" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C15" s="77">
         <v>0.19</v>
       </c>
       <c r="D15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E15" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>330i</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="78" t="s">
         <v>133</v>
       </c>
@@ -5245,100 +5429,148 @@
         <v>0.19</v>
       </c>
       <c r="D16" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E16" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>330i</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="78" t="s">
         <v>149</v>
       </c>
       <c r="B17" s="79" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C17" s="80">
         <v>0.185</v>
       </c>
       <c r="D17" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E17" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>530i</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="78" t="s">
         <v>149</v>
       </c>
       <c r="B18" s="79" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C18" s="80">
         <v>0.185</v>
       </c>
       <c r="D18" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E18" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>530i</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="75" t="s">
         <v>149</v>
       </c>
       <c r="B19" s="76" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C19" s="77">
         <v>0.185</v>
       </c>
       <c r="D19" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E19" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>530i</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="75" t="s">
         <v>149</v>
       </c>
       <c r="B20" s="76" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C20" s="77">
         <v>0.185</v>
       </c>
       <c r="D20" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E20" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>530i</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="75" t="s">
         <v>149</v>
       </c>
       <c r="B21" s="76" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C21" s="77">
         <v>0.185</v>
       </c>
       <c r="D21" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E21" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>530i</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="78" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B22" s="79" t="s">
         <v>204</v>
@@ -5347,15 +5579,23 @@
         <v>0.18</v>
       </c>
       <c r="D22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E22" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>X5</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>X5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="86" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B23" s="81">
         <v>48800</v>
@@ -5364,15 +5604,23 @@
         <v>0.185</v>
       </c>
       <c r="D23" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E23" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>330xi</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="87" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B24" s="83">
         <v>54400</v>
@@ -5381,15 +5629,23 @@
         <v>0.18</v>
       </c>
       <c r="D24" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E24" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>330xi</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="87" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B25" s="83">
         <v>65800</v>
@@ -5398,15 +5654,23 @@
         <v>0.19</v>
       </c>
       <c r="D25" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E25" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>530xi</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="87" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B26" s="83">
         <v>87000</v>
@@ -5415,15 +5679,23 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="D26" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E26" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>M550xi</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>M550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="86" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B27" s="81">
         <v>43200</v>
@@ -5432,15 +5704,23 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="D27" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E27" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>X1</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>X1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="87" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B28" s="83">
         <v>42700</v>
@@ -5449,15 +5729,23 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="D28" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E28" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>X2</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>X2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="86" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B29" s="81">
         <v>51250</v>
@@ -5466,15 +5754,23 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="D29" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E29" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v>X3</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>X3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="88" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B30" s="85">
         <v>60300</v>
@@ -5483,13 +5779,21 @@
         <v>0.17</v>
       </c>
       <c r="D30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E30" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>X3</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>X3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="86" t="s">
         <v>201</v>
       </c>
@@ -5500,15 +5804,23 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="D31" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E31" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>X4</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>X4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="87" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B32" s="83">
         <v>65300</v>
@@ -5517,13 +5829,21 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="D32" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E32" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F32" t="str">
+        <f t="shared" si="1"/>
+        <v>X5</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>X5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="86" t="s">
         <v>224</v>
       </c>
@@ -5534,146 +5854,218 @@
         <v>0.17</v>
       </c>
       <c r="D33" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E33" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F33" t="str">
+        <f t="shared" si="1"/>
+        <v>X7</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>X7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="89" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B34" s="90" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C34" s="91">
         <v>0.16500000000000001</v>
       </c>
       <c r="D34" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E34" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="65.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F34" t="str">
+        <f t="shared" si="1"/>
+        <v>540xi</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="2"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="65.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="92" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B35" s="93" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C35" s="94">
         <v>0.18</v>
       </c>
       <c r="D35" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E35" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F35" t="str">
+        <f t="shared" si="1"/>
+        <v>530xi</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="92" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B36" s="93" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C36" s="95">
         <v>0.185</v>
       </c>
       <c r="D36" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E36" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F36" t="str">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="92" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B37" s="93" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C37" s="95">
         <v>0.19500000000000001</v>
       </c>
       <c r="D37" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E37" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F37" t="str">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="92" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B38" s="93" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C38" s="95">
         <v>0.19500000000000001</v>
       </c>
       <c r="D38" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E38" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F38" t="str">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="92" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B39" s="93" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C39" s="94">
         <v>0.18</v>
       </c>
       <c r="D39" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E39" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F39" t="str">
+        <f t="shared" si="1"/>
+        <v>430xi</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="2"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="92" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B40" s="93" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C40" s="94">
         <v>0.14000000000000001</v>
       </c>
       <c r="D40" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E40" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F40" t="str">
+        <f t="shared" si="1"/>
+        <v>X5</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="2"/>
+        <v>X5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="49.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="92" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B41" s="93" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C41" s="94">
         <v>0.14000000000000001</v>
       </c>
       <c r="D41" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E41" t="s">
         <v>233</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="1"/>
+        <v>X5</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="2"/>
+        <v>X5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>